<commit_message>
moved relevant fnc from graphique to book & got started on sort unit tests
</commit_message>
<xml_diff>
--- a/CorrectionTP3.xlsx
+++ b/CorrectionTP3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walid Boulabiar\OneDrive - Cégep Limoilou\Cours IFT\IFT1004\IFT 1004 E2023\tps\TP3 E23\Livre\TP4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellecompte/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1CAA67-7D82-4641-A9DF-E4097AC52075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015" tabRatio="709"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="709" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP3" sheetId="48" r:id="rId1"/>
@@ -17,12 +18,25 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Barême</t>
   </si>
@@ -133,15 +147,31 @@
   </si>
   <si>
     <t>Option Aide, à propos</t>
+  </si>
+  <si>
+    <t>20 heures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexandre Dubeau et Gabriel Lecompte </t>
+  </si>
+  <si>
+    <t>111 091 011 (A.D) et  111 133 719 (G.L)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -220,24 +250,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -267,7 +298,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -284,9 +315,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -324,9 +355,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,7 +392,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,7 +427,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -569,66 +600,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="88.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="90.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="106.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="3.6640625" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="8"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="9"/>
+      <c r="D6" s="8"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
@@ -639,238 +679,238 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    </row>
+    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B21">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B22">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B23">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+    </row>
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
+    </row>
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B28">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B29">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B30">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+    </row>
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="B38" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="B39" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="B40" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="B41" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="7"/>
+      <c r="B43" s="11"/>
+    </row>
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
@@ -879,8 +919,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>